<commit_message>
jupyter notebook -> python
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Meu Drive\Programação\Python\Cartola FC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F321E5B-EF97-42A1-AEDB-4FF05CD58CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63074FBF-9711-4404-82C0-AB3CA7C1CD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,15 +377,36 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
+        <top style="thin">
           <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -406,36 +427,15 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -452,10 +452,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25863931-DC0D-47AD-AED9-0A600BEFDE34}" name="Tabela1" displayName="Tabela1" ref="A1:AM43" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25863931-DC0D-47AD-AED9-0A600BEFDE34}" name="Tabela1" displayName="Tabela1" ref="A1:AM43" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:AM43" xr:uid="{25863931-DC0D-47AD-AED9-0A600BEFDE34}"/>
   <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{B6CCF5DE-CAF1-4F3F-876E-FC687390F69A}" name="time" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{B6CCF5DE-CAF1-4F3F-876E-FC687390F69A}" name="time" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{39D8325F-5ACE-40A5-B78D-C1A8A2B8D6E8}" name="rodada38"/>
     <tableColumn id="3" xr3:uid="{13DEADD4-6D55-4441-A74E-81128049C93B}" name="rodada37"/>
     <tableColumn id="4" xr3:uid="{E5F96E8B-0092-46BE-B0E7-FEECB78B1F68}" name="rodada36"/>
@@ -823,7 +823,7 @@
   <dimension ref="A1:AM43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W37" sqref="A37:XFD37"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,7 +1575,7 @@
         <v>72.53</v>
       </c>
       <c r="J7">
-        <v>88.52</v>
+        <v>75.22</v>
       </c>
       <c r="K7">
         <v>84.54</v>

</xml_diff>